<commit_message>
Bài 29 - DataProvider - Data-Driven Testing
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/CRM.xlsx
+++ b/src/test/resources/testdata/CRM.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ANHTESTER\SeleniumJava\Course_SeleniumJava_062024\SeleniumTestNGParallel062024\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34CE5EE9-9872-438F-BD0A-584B61FF61BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1409B22D-B380-46B3-B8E5-8EB6717A5AE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" activeTab="1" xr2:uid="{FD95AF05-E084-470D-920C-8B2F56727A57}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" activeTab="2" xr2:uid="{FD95AF05-E084-470D-920C-8B2F56727A57}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="2" r:id="rId1"/>
     <sheet name="Customer" sheetId="3" r:id="rId2"/>
+    <sheet name="LoginDataProvider" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="34">
   <si>
     <t>Email</t>
   </si>
@@ -124,13 +125,28 @@
   </si>
   <si>
     <t>https://anhtester.com</t>
+  </si>
+  <si>
+    <t>admin2@example.com</t>
+  </si>
+  <si>
+    <t>admin3@example.com</t>
+  </si>
+  <si>
+    <t>admin4@example.com</t>
+  </si>
+  <si>
+    <t>admin5@example.com</t>
+  </si>
+  <si>
+    <t>123456</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="14"/>
       <color theme="1"/>
@@ -145,6 +161,15 @@
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="14"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="163"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -186,10 +211,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -205,8 +231,12 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -670,8 +700,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB6060B0-3001-4FEB-AA2D-485CE2C544E4}">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.3"/>
@@ -761,4 +791,77 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D0C629D-5C0B-48EC-9717-B82259E8BDC6}">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="24" customWidth="1"/>
+    <col min="2" max="2" width="11.4609375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A3" r:id="rId1" xr:uid="{E8DDE036-F351-4612-A11D-00023F29A977}"/>
+    <hyperlink ref="A4" r:id="rId2" xr:uid="{95256FFF-B065-4DF4-A7D8-F6DF63CE612E}"/>
+    <hyperlink ref="A6" r:id="rId3" xr:uid="{59103385-89DC-4AD7-8B87-A45054669788}"/>
+    <hyperlink ref="A5" r:id="rId4" xr:uid="{4B9275A7-BBC2-47AD-AE0C-F37022CF5740}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>